<commit_message>
QUIZ FUNCTION UNDER CONSTRUCTION
</commit_message>
<xml_diff>
--- a/TEST_DATA/test_logical.xlsx
+++ b/TEST_DATA/test_logical.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="41">
   <si>
     <t xml:space="preserve">SR_NO</t>
   </si>
@@ -89,6 +89,60 @@
   </si>
   <si>
     <t xml:space="preserve">Linux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPTITUDE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is the average of first five multiples of 12?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XYZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GHI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is the difference in the place value of 5 in the numeral 754853?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is the compound interest on Rs. 2500 for 2 years at rate of interest 4% per annum?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sohan started a business with a capital of Rs. 80000. After 6 months Mohan joined as a partner by investing Rs. 65000. After one year they earned total profit Rs. 20000. What is share of Sohan in the profit?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GENERAL_KNOWLEDGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Who was awarded the Lokmanya Tilak National Journalism Award in the year 2020?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Which district was awarded the Plastic Waste Management Award 2020?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Who was awarded the Prem Bhatia Award for political reporting for his work on issues related to the COVID19 pandemic?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WRITTEN_COMMUNICATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To complete the function of the written word, we require:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In business, the purpose of writing is mainly to:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In writing business letters, one has to be:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In a sentence, the verb agrees in number and person with its:</t>
   </si>
 </sst>
 </file>
@@ -195,13 +249,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="15.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="55.34"/>
@@ -335,6 +389,318 @@
       </c>
       <c r="H5" s="1" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>